<commit_message>
Test data at dev branch
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/RepoFinallyEclipse1/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AFFA2E-A0CA-7F49-82CB-E3CBB5136179}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107B8CE7-6A4C-2F46-BA27-D470267E4CD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -106,34 +106,34 @@
     <t>bingi18</t>
   </si>
   <si>
-    <t>z111</t>
-  </si>
-  <si>
-    <t>Z222</t>
-  </si>
-  <si>
-    <t>z333</t>
-  </si>
-  <si>
-    <t>z444</t>
-  </si>
-  <si>
-    <t>z555</t>
-  </si>
-  <si>
-    <t>z666</t>
-  </si>
-  <si>
-    <t>z777</t>
-  </si>
-  <si>
-    <t>z888</t>
-  </si>
-  <si>
-    <t>z999</t>
-  </si>
-  <si>
-    <t>z101010</t>
+    <t>z1111</t>
+  </si>
+  <si>
+    <t>Z2222</t>
+  </si>
+  <si>
+    <t>z3333</t>
+  </si>
+  <si>
+    <t>z4444</t>
+  </si>
+  <si>
+    <t>z5555</t>
+  </si>
+  <si>
+    <t>z6666</t>
+  </si>
+  <si>
+    <t>z7777</t>
+  </si>
+  <si>
+    <t>z8888</t>
+  </si>
+  <si>
+    <t>z9999</t>
+  </si>
+  <si>
+    <t>z10101010</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Test data into devA
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/RepoFinallyEclipse1/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107B8CE7-6A4C-2F46-BA27-D470267E4CD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F08379-CD69-BD4D-AAEB-5AA440FCA27D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -106,34 +106,34 @@
     <t>bingi18</t>
   </si>
   <si>
-    <t>z1111</t>
-  </si>
-  <si>
-    <t>Z2222</t>
-  </si>
-  <si>
-    <t>z3333</t>
-  </si>
-  <si>
-    <t>z4444</t>
-  </si>
-  <si>
-    <t>z5555</t>
-  </si>
-  <si>
-    <t>z6666</t>
-  </si>
-  <si>
-    <t>z7777</t>
-  </si>
-  <si>
-    <t>z8888</t>
-  </si>
-  <si>
-    <t>z9999</t>
-  </si>
-  <si>
-    <t>z10101010</t>
+    <t>z11111</t>
+  </si>
+  <si>
+    <t>Z22222</t>
+  </si>
+  <si>
+    <t>z33333</t>
+  </si>
+  <si>
+    <t>z44444</t>
+  </si>
+  <si>
+    <t>z55555</t>
+  </si>
+  <si>
+    <t>z66666</t>
+  </si>
+  <si>
+    <t>z77777</t>
+  </si>
+  <si>
+    <t>z88888</t>
+  </si>
+  <si>
+    <t>z99999</t>
+  </si>
+  <si>
+    <t>z1010101010</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
test data for DEVA
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/RepoFinallyEclipse1/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F08379-CD69-BD4D-AAEB-5AA440FCA27D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24396EFF-09C9-BF42-81F5-D5109F00DC0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -106,34 +106,34 @@
     <t>bingi18</t>
   </si>
   <si>
-    <t>z11111</t>
-  </si>
-  <si>
-    <t>Z22222</t>
-  </si>
-  <si>
-    <t>z33333</t>
-  </si>
-  <si>
-    <t>z44444</t>
-  </si>
-  <si>
-    <t>z55555</t>
-  </si>
-  <si>
-    <t>z66666</t>
-  </si>
-  <si>
-    <t>z77777</t>
-  </si>
-  <si>
-    <t>z88888</t>
-  </si>
-  <si>
-    <t>z99999</t>
-  </si>
-  <si>
-    <t>z1010101010</t>
+    <t>z111111</t>
+  </si>
+  <si>
+    <t>Z222222</t>
+  </si>
+  <si>
+    <t>z333333</t>
+  </si>
+  <si>
+    <t>z444444</t>
+  </si>
+  <si>
+    <t>z555555</t>
+  </si>
+  <si>
+    <t>z666666</t>
+  </si>
+  <si>
+    <t>z777777</t>
+  </si>
+  <si>
+    <t>z888888</t>
+  </si>
+  <si>
+    <t>z999999</t>
+  </si>
+  <si>
+    <t>z101010101010</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Commit for new test data
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/RepoFinallyEclipse1/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50679230-004C-894E-A388-5A35BD88BD39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55478AC9-BDC6-EC46-AA38-08B2E8A172EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -106,34 +106,34 @@
     <t>bingi18</t>
   </si>
   <si>
-    <t>z111111e</t>
-  </si>
-  <si>
-    <t>Z222222e</t>
-  </si>
-  <si>
-    <t>z333333e</t>
-  </si>
-  <si>
-    <t>z444444e</t>
-  </si>
-  <si>
-    <t>z555555e</t>
-  </si>
-  <si>
-    <t>z666666e</t>
-  </si>
-  <si>
-    <t>z777777e</t>
-  </si>
-  <si>
-    <t>z888888e</t>
-  </si>
-  <si>
-    <t>z999999e</t>
-  </si>
-  <si>
-    <t>z101010101010e</t>
+    <t>z111111e1</t>
+  </si>
+  <si>
+    <t>Z222222e2</t>
+  </si>
+  <si>
+    <t>z333333e3</t>
+  </si>
+  <si>
+    <t>z444444e4</t>
+  </si>
+  <si>
+    <t>z555555e5</t>
+  </si>
+  <si>
+    <t>z666666e6</t>
+  </si>
+  <si>
+    <t>z777777e7</t>
+  </si>
+  <si>
+    <t>z888888e8</t>
+  </si>
+  <si>
+    <t>z999999e9</t>
+  </si>
+  <si>
+    <t>z101010101010e10</t>
   </si>
 </sst>
 </file>

</xml_diff>